<commit_message>
Time Exec and avoid sleep in ScraperPopulation
</commit_message>
<xml_diff>
--- a/execution/TimeExec.xlsx
+++ b/execution/TimeExec.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antho\Documents\GitHub\angelmanDataExtract\execution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FB1C54B-7EF6-4CF7-8BF0-33D5DAA518B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{731A1B1E-4B51-4EED-BBB0-9C3D1C6ED90F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{ACAC62FC-BFF0-4D42-9379-C15EC8F20D90}"/>
   </bookViews>
@@ -431,7 +431,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -457,6 +457,9 @@
       <c r="B2">
         <v>106</v>
       </c>
+      <c r="C2">
+        <v>96</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
@@ -472,6 +475,9 @@
       </c>
       <c r="B4">
         <v>29</v>
+      </c>
+      <c r="C4">
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>